<commit_message>
charts for new data
</commit_message>
<xml_diff>
--- a/db/db_analysis/query_execution_times_4-8-2021-03-19.xlsx
+++ b/db/db_analysis/query_execution_times_4-8-2021-03-19.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dsghrg/workarea/work/zhaw_repos/s8/ba/releo/db/db_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2802E44D-0A7C-0146-91A5-37860EEC6311}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680D8A4C-5563-6443-BBD2-8E1ADF109EC1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="500" windowWidth="67860" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="940" yWindow="780" windowWidth="67860" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query_execution_times_4-8-2021-" sheetId="1" r:id="rId1"/>
@@ -14905,44 +14905,6 @@
           <cell r="F2">
             <v>37.7245452404022</v>
           </cell>
-          <cell r="H2">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="H3">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="H4">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="H5">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="H6">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="H7">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="H8">
-            <v>41.584400000000002</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="H9">
-            <v>41.584400000000002</v>
-          </cell>
         </row>
       </sheetData>
       <sheetData sheetId="2">
@@ -23169,6 +23131,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="89.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="17">
       <c r="A1" s="3" t="s">
@@ -23555,6 +23520,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="3" max="3" width="86.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="17">
       <c r="A1" s="3" t="s">
@@ -25857,7 +25825,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AK101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A2" workbookViewId="0">
       <selection activeCell="AK17" sqref="AK17:AK54"/>
     </sheetView>
   </sheetViews>
@@ -28313,7 +28281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AI101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
       <selection activeCell="N47" sqref="N47:N68"/>
     </sheetView>
   </sheetViews>

</xml_diff>